<commit_message>
back ke 1 baris .xlsx
</commit_message>
<xml_diff>
--- a/tes.xlsx
+++ b/tes.xlsx
@@ -14,15 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>tes ke tiga x</t>
-  </si>
-  <si>
-    <t>tes ke empat x</t>
-  </si>
-  <si>
-    <t>tes ke lima x</t>
+    <t>tes ke dua x</t>
   </si>
 </sst>
 </file>
@@ -38,7 +32,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -47,19 +41,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -76,11 +58,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,37 +365,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D10"/>
+  <dimension ref="A3:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rev .txt & .xlsx
</commit_message>
<xml_diff>
--- a/tes.xlsx
+++ b/tes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>tes ke dua x</t>
   </si>
@@ -32,7 +32,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -42,6 +42,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -58,9 +64,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,15 +372,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D3"/>
+  <dimension ref="A3:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -381,6 +388,14 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>